<commit_message>
asigning correct role to adj concatinated pronouns with dep role of NPOSTMOD & POSDEP
</commit_message>
<xml_diff>
--- a/adj_pronoun.xlsx
+++ b/adj_pronoun.xlsx
@@ -2800,7 +2800,7 @@
   <dimension ref="A1:F413"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F198" sqref="F198"/>
+      <selection activeCell="F103" sqref="F103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3205,7 +3205,7 @@
         <v>26000</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>45</v>
       </c>
@@ -4125,7 +4125,7 @@
         <v>31444</v>
       </c>
     </row>
-    <row r="67" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>139</v>
       </c>
@@ -4845,7 +4845,7 @@
         <v>34209</v>
       </c>
     </row>
-    <row r="103" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>202</v>
       </c>
@@ -5285,7 +5285,7 @@
         <v>35171</v>
       </c>
     </row>
-    <row r="125" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>239</v>
       </c>
@@ -5645,7 +5645,7 @@
         <v>47689</v>
       </c>
     </row>
-    <row r="143" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>267</v>
       </c>
@@ -5905,7 +5905,7 @@
         <v>37236</v>
       </c>
     </row>
-    <row r="156" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>283</v>
       </c>
@@ -6145,7 +6145,7 @@
         <v>38156</v>
       </c>
     </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>306</v>
       </c>
@@ -6205,7 +6205,7 @@
         <v>38209</v>
       </c>
     </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>310</v>
       </c>
@@ -6485,7 +6485,7 @@
         <v>38709</v>
       </c>
     </row>
-    <row r="185" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>333</v>
       </c>
@@ -6505,7 +6505,7 @@
         <v>38714</v>
       </c>
     </row>
-    <row r="186" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>335</v>
       </c>
@@ -6705,7 +6705,7 @@
         <v>38797</v>
       </c>
     </row>
-    <row r="196" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>348</v>
       </c>
@@ -6745,7 +6745,7 @@
         <v>39229</v>
       </c>
     </row>
-    <row r="198" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>350</v>
       </c>
@@ -6865,7 +6865,7 @@
         <v>39572</v>
       </c>
     </row>
-    <row r="204" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>362</v>
       </c>
@@ -7445,7 +7445,7 @@
         <v>42937</v>
       </c>
     </row>
-    <row r="233" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>401</v>
       </c>
@@ -7925,7 +7925,7 @@
         <v>49433</v>
       </c>
     </row>
-    <row r="257" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
         <v>429</v>
       </c>
@@ -8085,7 +8085,7 @@
         <v>50115</v>
       </c>
     </row>
-    <row r="265" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
         <v>438</v>
       </c>
@@ -8645,7 +8645,7 @@
         <v>52342</v>
       </c>
     </row>
-    <row r="293" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
         <v>479</v>
       </c>
@@ -8885,7 +8885,7 @@
         <v>53097</v>
       </c>
     </row>
-    <row r="305" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A305" t="s">
         <v>496</v>
       </c>
@@ -8905,7 +8905,7 @@
         <v>53266</v>
       </c>
     </row>
-    <row r="306" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A306" t="s">
         <v>498</v>
       </c>
@@ -8945,7 +8945,7 @@
         <v>53344</v>
       </c>
     </row>
-    <row r="308" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A308" t="s">
         <v>502</v>
       </c>
@@ -9145,7 +9145,7 @@
         <v>48522</v>
       </c>
     </row>
-    <row r="318" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A318" t="s">
         <v>518</v>
       </c>
@@ -9345,7 +9345,7 @@
         <v>54969</v>
       </c>
     </row>
-    <row r="328" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A328" t="s">
         <v>533</v>
       </c>
@@ -9645,7 +9645,7 @@
         <v>56184</v>
       </c>
     </row>
-    <row r="343" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A343" t="s">
         <v>550</v>
       </c>
@@ -9665,7 +9665,7 @@
         <v>56519</v>
       </c>
     </row>
-    <row r="344" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A344" t="s">
         <v>551</v>
       </c>
@@ -9805,7 +9805,7 @@
         <v>57566</v>
       </c>
     </row>
-    <row r="351" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A351" t="s">
         <v>561</v>
       </c>
@@ -9825,7 +9825,7 @@
         <v>58362</v>
       </c>
     </row>
-    <row r="352" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A352" t="s">
         <v>563</v>
       </c>
@@ -9845,7 +9845,7 @@
         <v>58443</v>
       </c>
     </row>
-    <row r="353" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A353" t="s">
         <v>565</v>
       </c>
@@ -9925,7 +9925,7 @@
         <v>58753</v>
       </c>
     </row>
-    <row r="357" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A357" t="s">
         <v>570</v>
       </c>
@@ -10065,7 +10065,7 @@
         <v>59063</v>
       </c>
     </row>
-    <row r="364" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A364" t="s">
         <v>580</v>
       </c>
@@ -10145,7 +10145,7 @@
         <v>26042</v>
       </c>
     </row>
-    <row r="368" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A368" t="s">
         <v>585</v>
       </c>
@@ -10205,7 +10205,7 @@
         <v>31250</v>
       </c>
     </row>
-    <row r="371" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A371" t="s">
         <v>590</v>
       </c>
@@ -10505,7 +10505,7 @@
         <v>36590</v>
       </c>
     </row>
-    <row r="386" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A386" t="s">
         <v>609</v>
       </c>
@@ -10745,7 +10745,7 @@
         <v>49796</v>
       </c>
     </row>
-    <row r="398" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A398" t="s">
         <v>623</v>
       </c>
@@ -10765,7 +10765,7 @@
         <v>50167</v>
       </c>
     </row>
-    <row r="399" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A399" t="s">
         <v>625</v>
       </c>
@@ -10805,7 +10805,7 @@
         <v>45561</v>
       </c>
     </row>
-    <row r="401" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A401" t="s">
         <v>629</v>
       </c>
@@ -10825,7 +10825,7 @@
         <v>52218</v>
       </c>
     </row>
-    <row r="402" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A402" t="s">
         <v>629</v>
       </c>
@@ -10845,7 +10845,7 @@
         <v>52218</v>
       </c>
     </row>
-    <row r="403" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A403" t="s">
         <v>631</v>
       </c>
@@ -10865,7 +10865,7 @@
         <v>52470</v>
       </c>
     </row>
-    <row r="404" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A404" t="s">
         <v>633</v>
       </c>
@@ -11069,7 +11069,7 @@
   <autoFilter ref="A1:F413">
     <filterColumn colId="4">
       <filters>
-        <filter val="MOS"/>
+        <filter val="POSDEP"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>